<commit_message>
feat(frontend): enhance UI and add data visualization
- update title and header for better user experience
- implement drag and drop functionality for file uploading
- add chart component to visualize data summaries
- improve status messages for user feedback

fix(agent): correct id generation and data handling

- fix bug in generating unique IDs for rows with missing data
- generate UUID for each row based on name and document
- fix some bugs in agent processing and data export

perf(agent): optimize merge operations and data analysis

- improve performance of dataframe merging
- optimize the way the agent does data analysis
</commit_message>
<xml_diff>
--- a/data/Ferramenta3  Claude.xlsx
+++ b/data/Ferramenta3  Claude.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielnichio/Desktop/Estudos/desafio-tech4humans/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA9CB7DB-D6A5-1B49-ADBA-30C551695994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3BD058-6F29-7745-BDFC-598EC1D9F614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{FCCDB15D-EE15-F548-B2C5-76FE5109C10A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="124">
   <si>
     <t>Nome</t>
   </si>
@@ -405,9 +405,6 @@
   </si>
   <si>
     <t>845.601.337-XX</t>
-  </si>
-  <si>
-    <t>112.233.554-XX</t>
   </si>
   <si>
     <t>Valor Total</t>
@@ -823,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43067FF2-8195-564B-90F0-68AF141AEED9}">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -841,7 +838,7 @@
         <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1498,9 +1495,7 @@
       <c r="A63" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>123</v>
-      </c>
+      <c r="B63" s="3"/>
       <c r="C63">
         <v>50</v>
       </c>

</xml_diff>